<commit_message>
Download printable reading plan
</commit_message>
<xml_diff>
--- a/WebStats.xlsx
+++ b/WebStats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TIM\Dev\MBP\Source\WebSite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{878BB8B2-0D91-4AE6-B0AF-8C0C1045BF68}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4678B097-7CC8-470C-A0C1-0288DA2D92CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-17295" yWindow="-1605" windowWidth="14910" windowHeight="13635" xr2:uid="{27BFC1CF-0A0F-4C52-BEAD-6F4936B2C4B4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{27BFC1CF-0A0F-4C52-BEAD-6F4936B2C4B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -209,10 +209,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$24</c:f>
+              <c:f>Sheet1!$A$2:$A$25</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="23"/>
+                <c:ptCount val="24"/>
                 <c:pt idx="0">
                   <c:v>43281</c:v>
                 </c:pt>
@@ -281,16 +281,19 @@
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>44135</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>44165</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$24</c:f>
+              <c:f>Sheet1!$B$2:$B$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="23"/>
+                <c:ptCount val="24"/>
                 <c:pt idx="0">
                   <c:v>353</c:v>
                 </c:pt>
@@ -359,6 +362,9 @@
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>15201</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>20906</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -414,10 +420,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$24</c:f>
+              <c:f>Sheet1!$A$2:$A$25</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="23"/>
+                <c:ptCount val="24"/>
                 <c:pt idx="0">
                   <c:v>43281</c:v>
                 </c:pt>
@@ -486,16 +492,19 @@
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>44135</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>44165</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$24</c:f>
+              <c:f>Sheet1!$C$2:$C$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="23"/>
+                <c:ptCount val="24"/>
                 <c:pt idx="0">
                   <c:v>261</c:v>
                 </c:pt>
@@ -564,6 +573,9 @@
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>9534</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>6694</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -748,6 +760,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="543005656"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="months"/>
@@ -1382,16 +1395,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>461962</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>404812</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>361950</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1716,10 +1729,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA48726D-97CC-484E-B54F-3295947CF754}">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1992,6 +2005,17 @@
         <v>9534</v>
       </c>
     </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>44165</v>
+      </c>
+      <c r="B25">
+        <v>20906</v>
+      </c>
+      <c r="C25">
+        <v>6694</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Updates to Ephesians 1
</commit_message>
<xml_diff>
--- a/WebStats.xlsx
+++ b/WebStats.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TIM\Dev\MBP\Source\WebSite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4678B097-7CC8-470C-A0C1-0288DA2D92CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E3579CF-A3F2-4C59-B162-1707335EC518}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{27BFC1CF-0A0F-4C52-BEAD-6F4936B2C4B4}"/>
   </bookViews>
@@ -207,12 +207,26 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$25</c:f>
+              <c:f>Sheet1!$A$2:$A$26</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="24"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="0">
                   <c:v>43281</c:v>
                 </c:pt>
@@ -284,16 +298,19 @@
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>44165</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>44196</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$25</c:f>
+              <c:f>Sheet1!$B$2:$B$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="24"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="0">
                   <c:v>353</c:v>
                 </c:pt>
@@ -365,6 +382,9 @@
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>20906</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>19769</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -418,12 +438,26 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$25</c:f>
+              <c:f>Sheet1!$A$2:$A$26</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="24"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="0">
                   <c:v>43281</c:v>
                 </c:pt>
@@ -495,16 +529,19 @@
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>44165</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>44196</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$25</c:f>
+              <c:f>Sheet1!$C$2:$C$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="24"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="0">
                   <c:v>261</c:v>
                 </c:pt>
@@ -576,6 +613,9 @@
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>6694</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>9545</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1729,10 +1769,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA48726D-97CC-484E-B54F-3295947CF754}">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2016,6 +2056,17 @@
         <v>6694</v>
       </c>
     </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>44196</v>
+      </c>
+      <c r="B26">
+        <v>19769</v>
+      </c>
+      <c r="C26">
+        <v>9545</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>